<commit_message>
got transmission times for phase 5 and phase 4
</commit_message>
<xml_diff>
--- a/phase5/charts.xlsx
+++ b/phase5/charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>percent</t>
   </si>
@@ -33,6 +33,21 @@
   </si>
   <si>
     <t>window size</t>
+  </si>
+  <si>
+    <t>phase 3</t>
+  </si>
+  <si>
+    <t>phase 4</t>
+  </si>
+  <si>
+    <t>phase 5</t>
+  </si>
+  <si>
+    <t>5% loss</t>
+  </si>
+  <si>
+    <t>10%error</t>
   </si>
 </sst>
 </file>
@@ -347,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:H9"/>
+  <dimension ref="C3:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -368,8 +383,17 @@
       <c r="H3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>1</v>
       </c>
@@ -382,8 +406,17 @@
       <c r="H4">
         <v>17240</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>15743</v>
+      </c>
+      <c r="M4">
+        <v>17336</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>2</v>
       </c>
@@ -396,8 +429,17 @@
       <c r="H5">
         <v>15091</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>28697</v>
+      </c>
+      <c r="M5">
+        <v>29538</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>5</v>
       </c>
@@ -411,7 +453,7 @@
         <v>14869</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>10</v>
       </c>
@@ -425,7 +467,7 @@
         <v>13089</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>20</v>
       </c>
@@ -439,7 +481,7 @@
         <v>36111</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="G9">
         <v>50</v>
       </c>

</xml_diff>